<commit_message>
find top5 estimated routes
</commit_message>
<xml_diff>
--- a/Results_CVPR/latest_results.xlsx
+++ b/Results_CVPR/latest_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhoumengjie/Desktop/route-finder/Results_CVPR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9905E594-B84F-1844-BC0B-20A178204D7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95030260-5BAB-C84F-B270-9700A8497506}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="460" windowWidth="24080" windowHeight="14400" activeTab="2" xr2:uid="{89BCA9C2-340F-1141-BF5E-EB747759752F}"/>
+    <workbookView xWindow="300" yWindow="460" windowWidth="24080" windowHeight="14400" xr2:uid="{89BCA9C2-340F-1141-BF5E-EB747759752F}"/>
   </bookViews>
   <sheets>
     <sheet name="uk vs nonuk" sheetId="1" r:id="rId1"/>
@@ -811,6 +811,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -921,7 +935,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1811,6 +1825,7 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1829,6 +1844,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1939,7 +1968,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5134,6 +5163,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5243,7 +5286,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6151,6 +6194,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6261,7 +6318,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7169,6 +7226,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7279,7 +7350,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8187,6 +8258,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -8297,7 +8382,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9229,6 +9314,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -9339,7 +9438,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15634,8 +15733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A229558-3438-F345-98A6-E7993FD6780F}">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16522,8 +16621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC30D49-EA90-6347-80FD-4785774765A2}">
   <dimension ref="A1:AJ75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="Q52" sqref="Q52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q62" sqref="Q62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>